<commit_message>
edit README file. 	add cost of socket panel.
</commit_message>
<xml_diff>
--- a/新屋装修.xlsx
+++ b/新屋装修.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\装修\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mine\Remodelling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696B951E-59C5-42F7-B828-F728ABA5B9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="电器" sheetId="1" r:id="rId1"/>
@@ -27,8 +26,9 @@
     <sheet name="杂项" sheetId="14" r:id="rId12"/>
     <sheet name=" 净洁具" sheetId="17" r:id="rId13"/>
     <sheet name=" 洁具五金" sheetId="15" r:id="rId14"/>
+    <sheet name="面板和漏电开关" sheetId="19" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="335">
   <si>
     <t>区域</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1222,13 +1222,141 @@
   </si>
   <si>
     <t>三楼厕所</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一开二三插座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1位双控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1位单控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2位单控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2位双控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3位单控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3位双控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4位单控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4位双控</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电视电脑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电脑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>380V63A漏电</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>380V32A4P空气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>25A1P单极</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220V63A漏电</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220V25A2P空气</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>防水双盒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315270.html#crumb-wrap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315586.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16A插座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100006258993.html#none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315570.html#crumb-wrap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011265498.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100005443888.html#crumb-wrap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100022723084.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315568.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315584.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315214.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315236.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.jd.com/100011315268.html#none</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://shop357702730.taobao.com/search.htm?orderType=coefp_desc&amp;viewType=grid&amp;keyword=%BF%D5%C6%F8%BF%AA%B9%D8&amp;lowPrice=&amp;highPrice=</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>链接</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1352,7 +1480,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1"/>
@@ -1380,6 +1508,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2224,11 +2358,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2238,7 +2372,7 @@
     <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="132.625" customWidth="1"/>
+    <col min="8" max="8" width="23.875" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2263,7 +2397,7 @@
       <c r="G1" t="s">
         <v>85</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2284,7 +2418,7 @@
         <v>6800</v>
       </c>
       <c r="G2" s="4"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="15" t="s">
         <v>84</v>
       </c>
     </row>
@@ -2302,7 +2436,7 @@
         <v>12491</v>
       </c>
       <c r="G3" s="4"/>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="15" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2320,7 +2454,7 @@
         <v>1799</v>
       </c>
       <c r="G4" s="4"/>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="15" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2335,7 +2469,7 @@
         <v>1399</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="15" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2353,7 +2487,7 @@
         <v>3139</v>
       </c>
       <c r="G6" s="4"/>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="15" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2374,7 +2508,7 @@
         <v>1479</v>
       </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="15" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2392,7 +2526,7 @@
         <v>3947</v>
       </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="15" t="s">
         <v>207</v>
       </c>
     </row>
@@ -2410,7 +2544,7 @@
         <v>1449</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="15" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2431,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="4"/>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="15" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2449,7 +2583,7 @@
         <v>634.85</v>
       </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2470,7 +2604,7 @@
         <v>0</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="15" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2488,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2506,7 +2640,7 @@
         <v>39</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2527,7 +2661,7 @@
         <v>3024.98</v>
       </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="15" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2548,7 +2682,7 @@
         <v>0</v>
       </c>
       <c r="G21" s="5"/>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="15" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2566,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="H22" s="1" t="s">
+      <c r="H22" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2587,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="4"/>
-      <c r="H24" s="1" t="s">
+      <c r="H24" s="15" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2605,7 +2739,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="4"/>
-      <c r="H25" s="1" t="s">
+      <c r="H25" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2623,7 +2757,7 @@
         <v>39</v>
       </c>
       <c r="G26" s="4"/>
-      <c r="H26" s="1" t="s">
+      <c r="H26" s="15" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2644,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="G28" s="4"/>
-      <c r="H28" s="1" t="s">
+      <c r="H28" s="15" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2662,7 +2796,7 @@
         <v>0</v>
       </c>
       <c r="G29" s="4"/>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="15" t="s">
         <v>47</v>
       </c>
     </row>
@@ -2680,12 +2814,12 @@
         <v>39</v>
       </c>
       <c r="G30" s="4"/>
-      <c r="H30" s="1" t="s">
+      <c r="H30" s="15" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H31" s="1"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
@@ -2704,12 +2838,12 @@
         <v>0</v>
       </c>
       <c r="G32" s="4"/>
-      <c r="H32" s="1" t="s">
+      <c r="H32" s="15" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H33" s="1"/>
+      <c r="H33" s="15"/>
     </row>
     <row r="34" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -2728,7 +2862,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="4"/>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="15" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2749,7 +2883,7 @@
         <v>3769</v>
       </c>
       <c r="G36" s="4"/>
-      <c r="H36" s="1" t="s">
+      <c r="H36" s="15" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2767,7 +2901,7 @@
         <v>0</v>
       </c>
       <c r="G37" s="4"/>
-      <c r="H37" s="1" t="s">
+      <c r="H37" s="15" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2785,12 +2919,12 @@
         <v>0</v>
       </c>
       <c r="G38" s="4"/>
-      <c r="H38" s="1" t="s">
+      <c r="H38" s="15" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H39" s="1"/>
+      <c r="H39" s="15"/>
     </row>
     <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
@@ -2809,7 +2943,7 @@
         <v>0</v>
       </c>
       <c r="G41" s="4"/>
-      <c r="H41" s="1" t="s">
+      <c r="H41" s="15" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2827,7 +2961,7 @@
         <v>62</v>
       </c>
       <c r="G42" s="4"/>
-      <c r="H42" s="1" t="s">
+      <c r="H42" s="15" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2848,7 +2982,7 @@
         <v>694</v>
       </c>
       <c r="G45" s="4"/>
-      <c r="H45" s="1" t="s">
+      <c r="H45" s="15" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2876,34 +3010,34 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1" location="detail" xr:uid="{8506D4EE-DB38-44D4-8565-780FD15BDBF9}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{FEF3E28F-3FF1-47E4-9DAF-7E4CF39CA06C}"/>
-    <hyperlink ref="H5" r:id="rId3" xr:uid="{73020584-59EF-4A4D-A758-B47722DEED16}"/>
-    <hyperlink ref="H8" r:id="rId4" location="crumb-wrap" xr:uid="{5BFCF57B-6E31-450F-924A-FA4D845CDD55}"/>
-    <hyperlink ref="H9" r:id="rId5" location="detail" xr:uid="{3D18E052-66E3-479C-A81C-169C0C370C4A}"/>
-    <hyperlink ref="H10" r:id="rId6" xr:uid="{42DB9B80-C638-45CC-ACA4-B0041D7B60D7}"/>
-    <hyperlink ref="H24" r:id="rId7" xr:uid="{4F4FE2A1-F90F-4A1D-8FC3-DD87933703FB}"/>
-    <hyperlink ref="H28" r:id="rId8" xr:uid="{F01D1BC6-6762-412F-B6CB-31B48F2F83F8}"/>
-    <hyperlink ref="H21" r:id="rId9" xr:uid="{939ABC7A-4B83-439F-B117-DA40EC0D506F}"/>
-    <hyperlink ref="H19" r:id="rId10" location="crumb-wrap" xr:uid="{50E8EAF6-A9F9-44D5-A10D-45EB3E9A645C}"/>
-    <hyperlink ref="H32" r:id="rId11" location="crumb-wrap" xr:uid="{498BDFAE-FB8B-40BE-8A0C-0713260DF695}"/>
-    <hyperlink ref="H37" r:id="rId12" location="crumb-wrap" xr:uid="{D3988598-4985-4777-8CED-9A785E154B9A}"/>
-    <hyperlink ref="H13" r:id="rId13" xr:uid="{FC734153-C60C-401E-9E85-2FDE095B2C9D}"/>
-    <hyperlink ref="H16" r:id="rId14" xr:uid="{9E7E049E-9CCE-4B1E-904C-B25C8FC6E943}"/>
-    <hyperlink ref="H22" r:id="rId15" xr:uid="{109E4862-F93F-47FA-A6C9-87BEB4B4024E}"/>
-    <hyperlink ref="H25" r:id="rId16" xr:uid="{FE87C1A9-E03D-466C-B2D7-EB65FE3F87A2}"/>
-    <hyperlink ref="H29" r:id="rId17" xr:uid="{F82A1993-C197-4246-BF30-F7CD3CF42939}"/>
-    <hyperlink ref="H38" r:id="rId18" xr:uid="{8EFEB03B-6C6F-4DE3-93C9-0C2D66544310}"/>
-    <hyperlink ref="H41" r:id="rId19" xr:uid="{971366BE-93D0-478D-A550-C779661F3DE5}"/>
-    <hyperlink ref="H42" r:id="rId20" xr:uid="{5C320B2C-2B42-4754-B2D1-E9627C866454}"/>
-    <hyperlink ref="H45" r:id="rId21" location="crumb-wrap" xr:uid="{8BDDEEDF-7597-49C5-BDFE-D680BDBF5FF1}"/>
-    <hyperlink ref="H6" r:id="rId22" location="detail" xr:uid="{3FEADCD1-7FB2-4856-8D12-7A85C4CC3822}"/>
-    <hyperlink ref="H2" r:id="rId23" location="detail" xr:uid="{76B26706-5402-43C9-874A-9CA89026389F}"/>
-    <hyperlink ref="H12" r:id="rId24" xr:uid="{08CFEAC5-800D-492E-8DC1-861FE0F4B067}"/>
-    <hyperlink ref="H15" r:id="rId25" xr:uid="{2037011D-C8AE-477D-9012-D59F63999851}"/>
-    <hyperlink ref="H34" r:id="rId26" xr:uid="{05BFC062-2737-4E5A-902E-ECAD533D63D8}"/>
-    <hyperlink ref="H30" r:id="rId27" xr:uid="{C1EF41D2-AD83-4CE1-B253-03A11DAEC728}"/>
-    <hyperlink ref="H36" r:id="rId28" xr:uid="{928D300E-56DE-443B-A20F-922D09E34E96}"/>
+    <hyperlink ref="H3" r:id="rId1" location="detail"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H5" r:id="rId3"/>
+    <hyperlink ref="H8" r:id="rId4" location="crumb-wrap"/>
+    <hyperlink ref="H9" r:id="rId5" location="detail"/>
+    <hyperlink ref="H10" r:id="rId6"/>
+    <hyperlink ref="H24" r:id="rId7"/>
+    <hyperlink ref="H28" r:id="rId8"/>
+    <hyperlink ref="H21" r:id="rId9"/>
+    <hyperlink ref="H19" r:id="rId10" location="crumb-wrap"/>
+    <hyperlink ref="H32" r:id="rId11" location="crumb-wrap"/>
+    <hyperlink ref="H37" r:id="rId12" location="crumb-wrap"/>
+    <hyperlink ref="H13" r:id="rId13"/>
+    <hyperlink ref="H16" r:id="rId14"/>
+    <hyperlink ref="H22" r:id="rId15"/>
+    <hyperlink ref="H25" r:id="rId16"/>
+    <hyperlink ref="H29" r:id="rId17"/>
+    <hyperlink ref="H38" r:id="rId18"/>
+    <hyperlink ref="H41" r:id="rId19"/>
+    <hyperlink ref="H42" r:id="rId20"/>
+    <hyperlink ref="H45" r:id="rId21" location="crumb-wrap"/>
+    <hyperlink ref="H6" r:id="rId22" location="detail"/>
+    <hyperlink ref="H2" r:id="rId23" location="detail"/>
+    <hyperlink ref="H12" r:id="rId24"/>
+    <hyperlink ref="H15" r:id="rId25"/>
+    <hyperlink ref="H34" r:id="rId26"/>
+    <hyperlink ref="H30" r:id="rId27"/>
+    <hyperlink ref="H36" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId29"/>
@@ -2911,7 +3045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BA7D41A-DEEA-48C7-BE58-3BC57F03FEA0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3051,11 +3185,11 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86BB10B5-3BB8-4C76-B405-155B335BC6BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3406,10 +3540,10 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" location="crumb-wrap" xr:uid="{ACEEF263-B691-48EB-AE6A-C40C5434FA21}"/>
-    <hyperlink ref="G19" r:id="rId2" xr:uid="{21633C77-8C4A-4928-A6EA-3219019774EF}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{CC838A3A-3FBF-4CCF-90FB-EA2357826D52}"/>
-    <hyperlink ref="G20" r:id="rId4" xr:uid="{DA1C8954-CC84-4B98-95D5-67680A2952EF}"/>
+    <hyperlink ref="G4" r:id="rId1" location="crumb-wrap"/>
+    <hyperlink ref="G19" r:id="rId2"/>
+    <hyperlink ref="G5" r:id="rId3"/>
+    <hyperlink ref="G20" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -3417,7 +3551,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A22AE47-2351-48E6-8751-649A31BBE403}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3687,7 +3821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2093F7-6BB6-4F6F-983A-629C0EAC18AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3919,10 +4053,10 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73A7CB05-9F2C-4DF0-95F3-270390B5B694}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -4644,24 +4778,390 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A24E19A-48EF-4D10-9DAA-3106E9BA28BA}">
-  <dimension ref="E2:H119"/>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="105.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2">
+        <v>85</v>
+      </c>
+      <c r="C2">
+        <v>13.6</v>
+      </c>
+      <c r="D2">
+        <f>C2*B2</f>
+        <v>1156</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>12.24</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D19" si="0">C3*B3</f>
+        <v>85.68</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>10.24</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>81.92</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>305</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>8.32</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>8.32</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>11.52</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>57.599999999999994</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>12.16</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>60.8</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>15.12</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>60.48</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>309</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>17.04</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>51.12</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>24.64</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>24.64</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>311</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>27.28</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>81.84</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>312</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>78</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>546</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>313</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>314</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>293.13</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>293.13</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>315</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>76.680000000000007</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>76.680000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>316</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>15.2</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>121.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>317</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>144.66999999999999</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>144.66999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>318</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>36.340000000000003</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>36.340000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>319</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>20.88</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>41.76</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="4">
+        <f>SUM(D2:D19)</f>
+        <v>2928.58</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" location="crumb-wrap"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3" location="none"/>
+    <hyperlink ref="E5" r:id="rId4" location="crumb-wrap"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E12" r:id="rId6" location="crumb-wrap"/>
+    <hyperlink ref="E7" r:id="rId7"/>
+    <hyperlink ref="E8" r:id="rId8"/>
+    <hyperlink ref="E9" r:id="rId9"/>
+    <hyperlink ref="E10" r:id="rId10"/>
+    <hyperlink ref="E11" r:id="rId11"/>
+    <hyperlink ref="E19" r:id="rId12" location="none"/>
+    <hyperlink ref="E14" r:id="rId13"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E2:H119"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="20.75" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="5:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="14" t="s">
         <v>78</v>
       </c>
       <c r="G2" s="3"/>
@@ -4671,7 +5171,7 @@
       <c r="E3" s="4">
         <v>1662.29</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="15" t="s">
         <v>68</v>
       </c>
       <c r="G3" s="3"/>
@@ -4698,7 +5198,7 @@
       <c r="H8" s="3"/>
     </row>
     <row r="15" spans="5:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F15" t="s">
+      <c r="F15" s="14" t="s">
         <v>79</v>
       </c>
     </row>
@@ -4706,18 +5206,18 @@
       <c r="E16" s="4">
         <v>198</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="15" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="18" spans="6:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F18" s="1"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="30" spans="6:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F30" s="1"/>
+      <c r="F30" s="15"/>
     </row>
     <row r="33" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F33" t="s">
+      <c r="F33" s="14" t="s">
         <v>126</v>
       </c>
     </row>
@@ -4725,15 +5225,15 @@
       <c r="E34" s="4">
         <v>145</v>
       </c>
-      <c r="F34" s="1" t="s">
+      <c r="F34" s="15" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="44" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F44" s="1"/>
+      <c r="F44" s="15"/>
     </row>
     <row r="50" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F50" t="s">
+      <c r="F50" s="14" t="s">
         <v>80</v>
       </c>
     </row>
@@ -4741,12 +5241,12 @@
       <c r="E51" s="4">
         <v>2999</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F51" s="15" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="73" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F73" t="s">
+      <c r="F73" s="14" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4754,12 +5254,12 @@
       <c r="E74" s="4">
         <v>1999</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F74" s="15" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="80" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F80" t="s">
+      <c r="F80" s="14" t="s">
         <v>127</v>
       </c>
     </row>
@@ -4767,12 +5267,12 @@
       <c r="E81" s="4">
         <v>172.69</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F81" s="15" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="91" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F91" t="s">
+      <c r="F91" s="14" t="s">
         <v>129</v>
       </c>
     </row>
@@ -4780,15 +5280,15 @@
       <c r="E92" s="4">
         <v>737.6</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="F92" s="15" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="101" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F101" s="1"/>
+      <c r="F101" s="15"/>
     </row>
     <row r="105" spans="5:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F105" t="s">
+      <c r="F105" s="14" t="s">
         <v>131</v>
       </c>
     </row>
@@ -4796,7 +5296,7 @@
       <c r="E106" s="4">
         <v>4871.95</v>
       </c>
-      <c r="F106" s="1" t="s">
+      <c r="F106" s="15" t="s">
         <v>132</v>
       </c>
     </row>
@@ -4805,21 +5305,21 @@
         <f>SUM(E3:E106)</f>
         <v>12785.529999999999</v>
       </c>
-      <c r="F119" t="s">
+      <c r="F119" s="14" t="s">
         <v>133</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{F0F08E30-E55A-4C53-9A23-4481660887A9}"/>
-    <hyperlink ref="F16" r:id="rId2" xr:uid="{A0BE13E6-2569-4DE4-8496-00BA19E6B92C}"/>
-    <hyperlink ref="F34" r:id="rId3" xr:uid="{FB43A9C7-9331-4866-B9DA-F74863EE6A39}"/>
-    <hyperlink ref="F51" r:id="rId4" location="crumb-wrap" xr:uid="{862ED588-B617-4115-85ED-462C0E9964F7}"/>
-    <hyperlink ref="F74" r:id="rId5" location="none" xr:uid="{9A903250-A9FF-44AB-97BC-565A59392490}"/>
-    <hyperlink ref="F81" r:id="rId6" xr:uid="{ADA7ABF1-8C11-47FD-98C0-D2AA79D4C141}"/>
-    <hyperlink ref="F92" r:id="rId7" xr:uid="{A4ED1676-D450-48EA-A935-B9831FC8299C}"/>
-    <hyperlink ref="F106" r:id="rId8" xr:uid="{D37B30B2-1262-4D06-81AF-28C386CA27C1}"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="F16" r:id="rId2"/>
+    <hyperlink ref="F34" r:id="rId3"/>
+    <hyperlink ref="F51" r:id="rId4" location="crumb-wrap"/>
+    <hyperlink ref="F74" r:id="rId5" location="none"/>
+    <hyperlink ref="F81" r:id="rId6"/>
+    <hyperlink ref="F92" r:id="rId7"/>
+    <hyperlink ref="F106" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId9"/>
@@ -4827,16 +5327,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17C921A-3F49-49EB-80E4-E2212EA4DFB1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F23" sqref="F22:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="110.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.625" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4849,8 +5349,8 @@
       <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
+      <c r="D1" s="3" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -4863,7 +5363,7 @@
       <c r="C2" s="4">
         <v>508</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="15" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4878,14 +5378,14 @@
         <f>B3*1000</f>
         <v>5260</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" location="detail" xr:uid="{CE182E04-53CD-4D5E-BA31-6109322A53A1}"/>
+    <hyperlink ref="D2" r:id="rId1" location="detail"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4893,7 +5393,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AAF8AC-CAA7-43E5-BA8F-AFDB8CBF270D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4941,7 +5441,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D1" r:id="rId1" xr:uid="{34F25A74-BD27-4A36-9799-4CA5BCE9DE89}"/>
+    <hyperlink ref="D1" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -4949,7 +5449,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC08422-23C5-4DD1-95BD-70E809BC65F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5005,11 +5505,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CBD4AFB-5004-47CD-91BE-C937A8BF6DB6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5048,11 +5548,11 @@
         <v>140</v>
       </c>
       <c r="E2">
-        <v>300</v>
+        <v>680</v>
       </c>
       <c r="F2">
         <f>SUM(C2:E2)</f>
-        <v>8108</v>
+        <v>8488</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -5199,7 +5699,7 @@
     <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F10" s="4">
         <f>SUM(F2:F9)</f>
-        <v>16441</v>
+        <v>16821</v>
       </c>
     </row>
   </sheetData>
@@ -5210,7 +5710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8430D2A0-3AE4-45CC-9B65-DA24C9B55D71}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5255,7 +5755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4877F31E-4B20-4D99-B57B-2050C09464E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5405,11 +5905,11 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A63133-0DC2-4812-B292-805F541C3FA2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>